<commit_message>
added outlier values in quality issues sheet
</commit_message>
<xml_diff>
--- a/Module-6-PY-Learning-4/Data/datasets.xlsx
+++ b/Module-6-PY-Learning-4/Data/datasets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\business\novo\project-novo-jan-2023\project-novo-python-pgm-masterclass\masterclass-learning-material\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F18E43-4633-4612-84DD-58E3B2FF5815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA68662-5EEF-4C67-AF7D-062410C2B5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{019ADB62-EE61-4DFB-8C8C-2C749F46E8FA}"/>
   </bookViews>
@@ -2263,7 +2263,7 @@
   <dimension ref="A1:R9995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2451,69 +2451,69 @@
     </row>
     <row r="4" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
-        <v>100004</v>
+        <v>100003</v>
       </c>
       <c r="B4" s="7">
-        <v>42318</v>
+        <v>42710</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>118</v>
+        <v>150</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>120</v>
+        <v>14</v>
       </c>
       <c r="J4" s="6">
-        <v>33311</v>
+        <v>90036</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O4" s="6">
-        <v>957.57749999999999</v>
+        <v>62</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="P4" s="6">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="6">
-        <v>0.45</v>
+        <v>0</v>
+      </c>
+      <c r="R4" s="6">
+        <v>6.8714000000000004</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
-        <v>100006</v>
+        <v>100004</v>
       </c>
       <c r="B5" s="7">
-        <v>41888</v>
+        <v>42318</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>4</v>
@@ -2522,54 +2522,48 @@
         <v>3</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="J5" s="6">
-        <v>90032</v>
+        <v>33311</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="O5" s="6">
-        <v>48.86</v>
+        <v>957.57749999999999</v>
       </c>
       <c r="P5" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="Q5" s="6">
-        <v>0</v>
-      </c>
-      <c r="R5" s="6">
-        <v>14.1694</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
-        <v>100006</v>
+        <v>100005</v>
       </c>
       <c r="B6" s="7">
-        <v>41888</v>
+        <v>42318</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>4</v>
@@ -2578,37 +2572,31 @@
         <v>3</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="J6" s="6">
-        <v>90032</v>
+        <v>33311</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="O6" s="6">
-        <v>48.86</v>
+        <v>55</v>
       </c>
       <c r="P6" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="R6" s="6">
-        <v>14.1694</v>
+        <v>2.5164</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2669,7 +2657,7 @@
     </row>
     <row r="8" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
-        <v>100011</v>
+        <v>100006</v>
       </c>
       <c r="B8" s="7">
         <v>41888</v>
@@ -2702,30 +2690,30 @@
         <v>124</v>
       </c>
       <c r="L8" s="6" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>40</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="O8" s="6">
-        <v>1706.184</v>
+        <v>48.86</v>
       </c>
       <c r="P8" s="6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q8" s="6">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="R8" s="6">
-        <v>85.309200000000004</v>
+        <v>14.1694</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6">
-        <v>100011</v>
+        <v>100006</v>
       </c>
       <c r="B9" s="7">
         <v>41888</v>
@@ -2758,30 +2746,30 @@
         <v>124</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="O9" s="6">
-        <v>1706.184</v>
+        <v>48.86</v>
       </c>
       <c r="P9" s="6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="Q9" s="6">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="R9" s="6">
-        <v>85.309200000000004</v>
+        <v>14.1694</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6">
-        <v>100011</v>
+        <v>100009</v>
       </c>
       <c r="B10" s="7">
         <v>41888</v>
@@ -2814,30 +2802,18 @@
         <v>124</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="O10" s="6">
-        <v>1706.184</v>
-      </c>
-      <c r="P10" s="6">
-        <v>9</v>
+        <v>18.504000000000001</v>
       </c>
       <c r="Q10" s="6">
         <v>0.2</v>
       </c>
-      <c r="R10" s="6">
-        <v>85.309200000000004</v>
-      </c>
     </row>
     <row r="11" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
-        <v>100011</v>
+        <v>100010</v>
       </c>
       <c r="B11" s="7">
         <v>41888</v>
@@ -2870,42 +2846,39 @@
         <v>124</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="O11" s="6">
-        <v>1706.184</v>
+        <v>114.9</v>
       </c>
       <c r="P11" s="6">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q11" s="6">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="R11" s="6">
-        <v>85.309200000000004</v>
+        <v>34.47</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6">
-        <v>100024</v>
+        <v>100011</v>
       </c>
       <c r="B12" s="7">
-        <v>42932</v>
+        <v>41888</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>4</v>
@@ -2914,48 +2887,54 @@
         <v>3</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>128</v>
+        <v>14</v>
       </c>
       <c r="J12" s="6">
-        <v>19140</v>
+        <v>90032</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>130</v>
+        <v>36</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="O12" s="6">
-        <v>71.372</v>
+        <v>1706.184</v>
       </c>
       <c r="P12" s="6">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="Q12" s="6">
-        <v>0.3</v>
+        <v>0.2</v>
+      </c>
+      <c r="R12" s="6">
+        <v>85.309200000000004</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
-        <v>100025</v>
+        <v>100011</v>
       </c>
       <c r="B13" s="7">
-        <v>42272</v>
+        <v>41888</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>4</v>
@@ -2964,19 +2943,19 @@
         <v>3</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>134</v>
+        <v>14</v>
       </c>
       <c r="J13" s="6">
-        <v>84057</v>
+        <v>90032</v>
       </c>
       <c r="K13" s="6" t="s">
         <v>124</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>35</v>
@@ -2985,30 +2964,33 @@
         <v>34</v>
       </c>
       <c r="O13" s="6">
-        <v>1044.6300000000001</v>
+        <v>1706.184</v>
+      </c>
+      <c r="P13" s="6">
+        <v>9</v>
       </c>
       <c r="Q13" s="6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="R13" s="6">
-        <v>240.26490000000001</v>
+        <v>85.309200000000004</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
-        <v>100028</v>
+        <v>100011</v>
       </c>
       <c r="B14" s="7">
-        <v>42264</v>
+        <v>41888</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>4</v>
@@ -3017,45 +2999,54 @@
         <v>3</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>128</v>
+        <v>14</v>
       </c>
       <c r="J14" s="6">
-        <v>19140</v>
+        <v>90032</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>35</v>
       </c>
+      <c r="N14" s="6" t="s">
+        <v>34</v>
+      </c>
       <c r="O14" s="6">
-        <v>3083.43</v>
+        <v>1706.184</v>
+      </c>
+      <c r="P14" s="6">
+        <v>9</v>
       </c>
       <c r="Q14" s="6">
-        <v>0.5</v>
+        <v>0.2</v>
+      </c>
+      <c r="R14" s="6">
+        <v>85.309200000000004</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
-        <v>100030</v>
+        <v>100011</v>
       </c>
       <c r="B15" s="7">
-        <v>42264</v>
+        <v>41888</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>4</v>
@@ -3064,104 +3055,101 @@
         <v>3</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>128</v>
+        <v>14</v>
       </c>
       <c r="J15" s="6">
-        <v>19140</v>
+        <v>90032</v>
       </c>
       <c r="K15" s="6" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>138</v>
+        <v>36</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>35</v>
       </c>
       <c r="N15" s="6" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="O15" s="6">
-        <v>124.2</v>
+        <v>1706.184</v>
+      </c>
+      <c r="P15" s="6">
+        <v>9</v>
       </c>
       <c r="Q15" s="6">
         <v>0.2</v>
       </c>
       <c r="R15" s="6">
-        <v>15.525</v>
+        <v>85.309200000000004</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
-        <v>100037</v>
+        <v>100015</v>
       </c>
       <c r="B16" s="7">
-        <v>42712</v>
+        <v>42330</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>141</v>
+        <v>7</v>
       </c>
       <c r="I16" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J16" s="6">
-        <v>75080</v>
+        <v>76106</v>
       </c>
       <c r="K16" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>52</v>
+        <v>153</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="O16" s="6">
-        <v>190.92</v>
-      </c>
-      <c r="P16" s="6">
-        <v>5</v>
+        <v>68.81</v>
       </c>
       <c r="Q16" s="6">
-        <v>0.6</v>
-      </c>
-      <c r="R16" s="6">
-        <v>-147.96299999999999</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
-        <v>100039</v>
+        <v>100016</v>
       </c>
       <c r="B17" s="7">
-        <v>42365</v>
+        <v>42330</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="F17" s="6" t="s">
         <v>145</v>
@@ -3170,145 +3158,157 @@
         <v>3</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>146</v>
+        <v>7</v>
       </c>
       <c r="I17" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J17" s="6">
-        <v>77041</v>
+        <v>76106</v>
       </c>
       <c r="K17" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L17" s="6" t="s">
-        <v>147</v>
+        <v>154</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="O17" s="6">
-        <v>532.39919999999995</v>
+        <v>2.544</v>
+      </c>
+      <c r="P17" s="6">
+        <v>3</v>
       </c>
       <c r="Q17" s="6">
-        <v>0.32</v>
+        <v>0.8</v>
+      </c>
+      <c r="R17" s="6">
+        <v>-3.8159999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
-        <v>100040</v>
+        <v>100017</v>
       </c>
       <c r="B18" s="7">
-        <v>42365</v>
+        <v>41954</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>145</v>
+        <v>4</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
       <c r="J18" s="6">
-        <v>77041</v>
+        <v>53711</v>
       </c>
       <c r="K18" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>148</v>
+        <v>159</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="O18" s="6">
-        <v>212.05799999999999</v>
+        <v>665.88</v>
       </c>
       <c r="P18" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q18" s="6">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="R18" s="6">
-        <v>-15.147</v>
+        <v>13.317600000000001</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
-        <v>100003</v>
+        <v>100018</v>
       </c>
       <c r="B19" s="7">
-        <v>42710</v>
+        <v>41772</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>111</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>14</v>
+        <v>134</v>
       </c>
       <c r="J19" s="6">
-        <v>90036</v>
+        <v>84084</v>
       </c>
       <c r="K19" s="6" t="s">
         <v>124</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="P19" s="6">
-        <v>2</v>
+        <v>163</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O19" s="6">
+        <v>55.5</v>
       </c>
       <c r="Q19" s="6">
         <v>0</v>
       </c>
-      <c r="R19" s="6">
-        <v>6.8714000000000004</v>
-      </c>
     </row>
     <row r="20" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
-        <v>100005</v>
+        <v>100019</v>
       </c>
       <c r="B20" s="7">
-        <v>42318</v>
+        <v>41878</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>117</v>
+        <v>164</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>118</v>
+        <v>165</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>4</v>
@@ -3317,48 +3317,48 @@
         <v>3</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>120</v>
+        <v>14</v>
       </c>
       <c r="J20" s="6">
-        <v>33311</v>
+        <v>94109</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="L20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>55</v>
+        <v>167</v>
+      </c>
+      <c r="M20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O20" s="6">
+        <v>8.56</v>
       </c>
       <c r="P20" s="6">
         <v>2</v>
       </c>
       <c r="Q20" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="R20" s="6">
-        <v>2.5164</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
-        <v>100009</v>
+        <v>100020</v>
       </c>
       <c r="B21" s="7">
-        <v>41888</v>
+        <v>41878</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>122</v>
+        <v>165</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>4</v>
@@ -3367,22 +3367,22 @@
         <v>3</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="I21" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J21" s="6">
-        <v>90032</v>
+        <v>94109</v>
       </c>
       <c r="K21" s="6" t="s">
         <v>124</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>45</v>
+        <v>204</v>
       </c>
       <c r="O21" s="6">
-        <v>18.504000000000001</v>
+        <v>213.48</v>
       </c>
       <c r="Q21" s="6">
         <v>0.2</v>
@@ -3390,19 +3390,19 @@
     </row>
     <row r="22" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
-        <v>100010</v>
+        <v>100021</v>
       </c>
       <c r="B22" s="7">
-        <v>41888</v>
+        <v>41878</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>121</v>
+        <v>164</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>122</v>
+        <v>165</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>4</v>
@@ -3411,119 +3411,131 @@
         <v>3</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>123</v>
+        <v>166</v>
       </c>
       <c r="I22" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J22" s="6">
-        <v>90032</v>
+        <v>94109</v>
       </c>
       <c r="K22" s="6" t="s">
         <v>124</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>41</v>
+        <v>168</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="O22" s="6">
-        <v>114.9</v>
+        <v>22.72</v>
       </c>
       <c r="P22" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q22" s="6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="R22" s="6">
-        <v>34.47</v>
+        <v>7.3840000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
-        <v>100015</v>
+        <v>100021</v>
       </c>
       <c r="B23" s="7">
-        <v>42330</v>
+        <v>41878</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>145</v>
+        <v>4</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J23" s="6">
-        <v>76106</v>
+        <v>94109</v>
       </c>
       <c r="K23" s="6" t="s">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="M23" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="N23" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="O23" s="6">
-        <v>68.81</v>
+        <v>22.72</v>
+      </c>
+      <c r="P23" s="6">
+        <v>3</v>
       </c>
       <c r="Q23" s="6">
-        <v>0.8</v>
+        <v>0.2</v>
+      </c>
+      <c r="R23" s="6">
+        <v>7.3840000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
-        <v>100016</v>
+        <v>100021</v>
       </c>
       <c r="B24" s="7">
-        <v>42330</v>
+        <v>41878</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>145</v>
+        <v>4</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J24" s="6">
-        <v>76106</v>
+        <v>94109</v>
       </c>
       <c r="K24" s="6" t="s">
-        <v>0</v>
+        <v>124</v>
       </c>
       <c r="L24" s="6" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="M24" s="6" t="s">
         <v>40</v>
@@ -3532,33 +3544,33 @@
         <v>44</v>
       </c>
       <c r="O24" s="6">
-        <v>2.544</v>
+        <v>22.72</v>
       </c>
       <c r="P24" s="6">
         <v>3</v>
       </c>
       <c r="Q24" s="6">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="R24" s="6">
-        <v>-3.8159999999999998</v>
+        <v>7.3840000000000003</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
-        <v>100017</v>
+        <v>100024</v>
       </c>
       <c r="B25" s="7">
-        <v>41954</v>
+        <v>42932</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>4</v>
@@ -3567,54 +3579,48 @@
         <v>3</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="J25" s="6">
-        <v>53711</v>
+        <v>19140</v>
       </c>
       <c r="K25" s="6" t="s">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="M25" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="O25" s="6">
-        <v>665.88</v>
+        <v>71.372</v>
       </c>
       <c r="P25" s="6">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Q25" s="6">
-        <v>0</v>
-      </c>
-      <c r="R25" s="6">
-        <v>13.317600000000001</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
-        <v>100018</v>
+        <v>100025</v>
       </c>
       <c r="B26" s="7">
-        <v>41772</v>
+        <v>42272</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>160</v>
+        <v>131</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>161</v>
+        <v>132</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>4</v>
@@ -3623,45 +3629,51 @@
         <v>3</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>162</v>
+        <v>133</v>
       </c>
       <c r="I26" s="6" t="s">
         <v>134</v>
       </c>
       <c r="J26" s="6">
-        <v>84084</v>
+        <v>84057</v>
       </c>
       <c r="K26" s="6" t="s">
         <v>124</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>163</v>
+        <v>58</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="O26" s="6">
-        <v>55.5</v>
+        <v>1044.6300000000001</v>
       </c>
       <c r="Q26" s="6">
         <v>0</v>
       </c>
+      <c r="R26" s="6">
+        <v>240.26490000000001</v>
+      </c>
     </row>
     <row r="27" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
-        <v>100019</v>
+        <v>100026</v>
       </c>
       <c r="B27" s="7">
-        <v>41878</v>
+        <v>42385</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>111</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>4</v>
@@ -3670,48 +3682,51 @@
         <v>3</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>166</v>
+        <v>123</v>
       </c>
       <c r="I27" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J27" s="6">
-        <v>94109</v>
+        <v>90049</v>
       </c>
       <c r="K27" s="6" t="s">
         <v>124</v>
       </c>
       <c r="L27" s="6" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="M27" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O27" s="6">
-        <v>8.56</v>
+      <c r="N27" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="P27" s="6">
         <v>2</v>
       </c>
       <c r="Q27" s="6">
-        <v>0</v>
+        <v>0.2</v>
+      </c>
+      <c r="R27" s="6">
+        <v>4.2224000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6">
-        <v>100021</v>
+        <v>100027</v>
       </c>
       <c r="B28" s="7">
-        <v>41878</v>
+        <v>42385</v>
       </c>
       <c r="C28" s="6" t="s">
         <v>111</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>4</v>
@@ -3720,54 +3735,48 @@
         <v>3</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>166</v>
+        <v>123</v>
       </c>
       <c r="I28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J28" s="6">
-        <v>94109</v>
+        <v>90049</v>
       </c>
       <c r="K28" s="6" t="s">
         <v>124</v>
       </c>
       <c r="L28" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>40</v>
+        <v>205</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>44</v>
+        <v>206</v>
       </c>
       <c r="O28" s="6">
-        <v>22.72</v>
-      </c>
-      <c r="P28" s="6">
-        <v>3</v>
+        <v>90.57</v>
       </c>
       <c r="Q28" s="6">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="R28" s="6">
-        <v>7.3840000000000003</v>
+        <v>11.774100000000001</v>
       </c>
     </row>
     <row r="29" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
-        <v>100021</v>
+        <v>100028</v>
       </c>
       <c r="B29" s="7">
-        <v>41878</v>
+        <v>42264</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>4</v>
@@ -3776,54 +3785,45 @@
         <v>3</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
       <c r="J29" s="6">
-        <v>94109</v>
+        <v>19140</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="M29" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="O29" s="6">
-        <v>22.72</v>
-      </c>
-      <c r="P29" s="6">
-        <v>3</v>
+        <v>300083.43</v>
       </c>
       <c r="Q29" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="R29" s="6">
-        <v>7.3840000000000003</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6">
-        <v>100021</v>
+        <v>100029</v>
       </c>
       <c r="B30" s="7">
-        <v>41878</v>
+        <v>42264</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>4</v>
@@ -3832,19 +3832,19 @@
         <v>3</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
       <c r="J30" s="6">
-        <v>94109</v>
+        <v>19140</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="M30" s="6" t="s">
         <v>40</v>
@@ -3852,34 +3852,31 @@
       <c r="N30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="O30" s="6">
-        <v>22.72</v>
-      </c>
       <c r="P30" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q30" s="6">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="R30" s="6">
-        <v>7.3840000000000003</v>
+        <v>-7.0532000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
-        <v>100026</v>
+        <v>100030</v>
       </c>
       <c r="B31" s="7">
-        <v>42385</v>
+        <v>42264</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>4</v>
@@ -3888,39 +3885,39 @@
         <v>3</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>14</v>
+        <v>128</v>
       </c>
       <c r="J31" s="6">
-        <v>90049</v>
+        <v>19140</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="P31" s="6">
-        <v>2</v>
+        <v>52</v>
+      </c>
+      <c r="O31" s="6">
+        <v>124.2</v>
       </c>
       <c r="Q31" s="6">
         <v>0.2</v>
       </c>
       <c r="R31" s="6">
-        <v>4.2224000000000004</v>
+        <v>15.525</v>
       </c>
     </row>
     <row r="32" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
-        <v>100029</v>
+        <v>100031</v>
       </c>
       <c r="B32" s="7">
         <v>42264</v>
@@ -3953,27 +3950,24 @@
         <v>129</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="M32" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="N32" s="6" t="s">
-        <v>44</v>
+      <c r="O32" s="6">
+        <v>3.2639999999999998</v>
       </c>
       <c r="P32" s="6">
         <v>2</v>
       </c>
       <c r="Q32" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="R32" s="6">
-        <v>-7.0532000000000004</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
-        <v>100031</v>
+        <v>100032</v>
       </c>
       <c r="B33" s="7">
         <v>42264</v>
@@ -4006,16 +4000,13 @@
         <v>129</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="M33" s="6" t="s">
         <v>40</v>
       </c>
       <c r="O33" s="6">
-        <v>3.2639999999999998</v>
-      </c>
-      <c r="P33" s="6">
-        <v>2</v>
+        <v>86.304000000000002</v>
       </c>
       <c r="Q33" s="6">
         <v>0.2</v>
@@ -4023,7 +4014,7 @@
     </row>
     <row r="34" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="6">
-        <v>100032</v>
+        <v>100033</v>
       </c>
       <c r="B34" s="7">
         <v>42264</v>
@@ -4056,21 +4047,30 @@
         <v>129</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="M34" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="N34" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="O34" s="6">
-        <v>86.304000000000002</v>
+        <v>6.8579999999999997</v>
+      </c>
+      <c r="P34" s="6">
+        <v>6</v>
       </c>
       <c r="Q34" s="6">
-        <v>0.2</v>
+        <v>0.7</v>
+      </c>
+      <c r="R34" s="6">
+        <v>-5.7149999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
-        <v>100033</v>
+        <v>100034</v>
       </c>
       <c r="B35" s="7">
         <v>42264</v>
@@ -4103,530 +4103,548 @@
         <v>129</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="M35" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="N35" s="6" t="s">
-        <v>44</v>
-      </c>
       <c r="O35" s="6">
-        <v>6.8579999999999997</v>
-      </c>
-      <c r="P35" s="6">
-        <v>6</v>
+        <v>15.76</v>
       </c>
       <c r="Q35" s="6">
-        <v>0.7</v>
-      </c>
-      <c r="R35" s="6">
-        <v>-5.7149999999999999</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6">
-        <v>100034</v>
+        <v>100035</v>
       </c>
       <c r="B36" s="7">
-        <v>42264</v>
+        <v>43027</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>135</v>
+        <v>177</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>136</v>
+        <v>178</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>4</v>
+        <v>145</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>128</v>
+        <v>6</v>
       </c>
       <c r="J36" s="6">
-        <v>19140</v>
+        <v>77095</v>
       </c>
       <c r="K36" s="6" t="s">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="M36" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="N36" s="6" t="s">
+        <v>180</v>
+      </c>
       <c r="O36" s="6">
-        <v>15.76</v>
+        <v>29.472000000000001</v>
       </c>
       <c r="Q36" s="6">
         <v>0.2</v>
       </c>
+      <c r="R36" s="6">
+        <v>9.9467999999999996</v>
+      </c>
     </row>
     <row r="37" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6">
-        <v>100035</v>
+        <v>100036</v>
       </c>
       <c r="B37" s="7">
-        <v>43027</v>
+        <v>42712</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>177</v>
+        <v>139</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I37" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J37" s="6">
-        <v>77095</v>
+        <v>75080</v>
       </c>
       <c r="K37" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L37" s="6" t="s">
-        <v>179</v>
+        <v>207</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>40</v>
+        <v>208</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>180</v>
+        <v>31</v>
       </c>
       <c r="O37" s="6">
-        <v>29.472000000000001</v>
+        <v>109700.54399999999</v>
+      </c>
+      <c r="P37" s="6">
+        <v>7</v>
       </c>
       <c r="Q37" s="6">
         <v>0.2</v>
       </c>
       <c r="R37" s="6">
-        <v>9.9467999999999996</v>
+        <v>123.47369999999999</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6">
-        <v>100038</v>
+        <v>100037</v>
       </c>
       <c r="B38" s="7">
-        <v>42365</v>
+        <v>42712</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="I38" s="6" t="s">
         <v>6</v>
       </c>
       <c r="J38" s="6">
-        <v>77041</v>
+        <v>75080</v>
       </c>
       <c r="K38" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L38" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="M38" s="6" t="s">
-        <v>40</v>
+        <v>142</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>182</v>
+        <v>52</v>
+      </c>
+      <c r="O38" s="6">
+        <v>190.92</v>
       </c>
       <c r="P38" s="6">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="Q38" s="6">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="R38" s="6">
-        <v>35.414999999999999</v>
+        <v>-147.96299999999999</v>
       </c>
     </row>
     <row r="39" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6">
-        <v>100043</v>
+        <v>100038</v>
       </c>
       <c r="B39" s="7">
-        <v>42568</v>
+        <v>42365</v>
       </c>
       <c r="C39" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>184</v>
+        <v>144</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J39" s="6">
-        <v>90049</v>
+        <v>77041</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>124</v>
+        <v>0</v>
       </c>
       <c r="L39" s="6" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="M39" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O39" s="6">
-        <v>77.88</v>
+      <c r="N39" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="P39" s="6">
+        <v>9</v>
       </c>
       <c r="Q39" s="6">
-        <v>0</v>
+        <v>0.2</v>
+      </c>
+      <c r="R39" s="6">
+        <v>35.414999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6">
-        <v>100044</v>
+        <v>100039</v>
       </c>
       <c r="B40" s="7">
-        <v>42997</v>
+        <v>42365</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>186</v>
+        <v>143</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>187</v>
+        <v>144</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="G40" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>188</v>
+        <v>146</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>120</v>
+        <v>6</v>
       </c>
       <c r="J40" s="6">
-        <v>32935</v>
+        <v>77041</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="L40" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="M40" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="N40" s="6" t="s">
-        <v>55</v>
+        <v>147</v>
       </c>
       <c r="O40" s="6">
-        <v>95.616</v>
+        <v>532.39919999999995</v>
       </c>
       <c r="Q40" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="R40" s="6">
-        <v>9.5616000000000003</v>
+        <v>0.32</v>
       </c>
     </row>
     <row r="41" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6">
-        <v>100046</v>
+        <v>100040</v>
       </c>
       <c r="B41" s="7">
-        <v>42440</v>
+        <v>42365</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>190</v>
+        <v>143</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>191</v>
+        <v>144</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="G41" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>192</v>
+        <v>146</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>193</v>
+        <v>6</v>
       </c>
       <c r="J41" s="6">
-        <v>55122</v>
+        <v>77041</v>
       </c>
       <c r="K41" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>194</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>40</v>
+        <v>148</v>
+      </c>
+      <c r="N41" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="O41" s="6">
-        <v>17.46</v>
+        <v>212.05799999999999</v>
+      </c>
+      <c r="P41" s="6">
+        <v>3</v>
       </c>
       <c r="Q41" s="6">
-        <v>0</v>
+        <v>0.3</v>
+      </c>
+      <c r="R41" s="6">
+        <v>-15.147</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6">
-        <v>100047</v>
+        <v>100041</v>
       </c>
       <c r="B42" s="7">
-        <v>41932</v>
+        <v>42365</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>195</v>
+        <v>143</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>196</v>
+        <v>144</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>4</v>
+        <v>145</v>
       </c>
       <c r="G42" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>197</v>
+        <v>146</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J42" s="6">
-        <v>48185</v>
+        <v>77041</v>
       </c>
       <c r="K42" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>198</v>
+        <v>209</v>
       </c>
       <c r="M42" s="6" t="s">
-        <v>40</v>
+        <v>208</v>
       </c>
       <c r="O42" s="6">
-        <v>211.96</v>
+        <v>371.16800000000001</v>
+      </c>
+      <c r="P42" s="6">
+        <v>4</v>
       </c>
       <c r="Q42" s="6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="43" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6">
-        <v>100050</v>
+        <v>100042</v>
       </c>
       <c r="B43" s="7">
-        <v>42112</v>
+        <v>42988</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>199</v>
+        <v>210</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G43" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>201</v>
+        <v>212</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>202</v>
+        <v>17</v>
       </c>
       <c r="J43" s="6">
-        <v>47150</v>
+        <v>60540</v>
       </c>
       <c r="K43" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L43" s="6" t="s">
-        <v>203</v>
+        <v>213</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>208</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="O43" s="6">
-        <v>38.22</v>
+        <v>31</v>
+      </c>
+      <c r="P43" s="6">
+        <v>4</v>
       </c>
       <c r="Q43" s="6">
-        <v>0</v>
+        <v>0.2</v>
+      </c>
+      <c r="R43" s="6">
+        <v>16.5564</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6">
-        <v>100020</v>
+        <v>100043</v>
       </c>
       <c r="B44" s="7">
-        <v>41878</v>
+        <v>42568</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>164</v>
+        <v>183</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>165</v>
+        <v>184</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>166</v>
+        <v>123</v>
       </c>
       <c r="I44" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J44" s="6">
-        <v>94109</v>
+        <v>90049</v>
       </c>
       <c r="K44" s="6" t="s">
         <v>124</v>
       </c>
       <c r="L44" s="6" t="s">
-        <v>204</v>
+        <v>185</v>
+      </c>
+      <c r="M44" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="O44" s="6">
-        <v>213.48</v>
+        <v>77.88</v>
       </c>
       <c r="Q44" s="6">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6">
-        <v>100027</v>
+        <v>100044</v>
       </c>
       <c r="B45" s="7">
-        <v>42385</v>
+        <v>42997</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G45" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>123</v>
+        <v>188</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="J45" s="6">
-        <v>90049</v>
+        <v>32935</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>205</v>
+        <v>189</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>206</v>
+        <v>55</v>
       </c>
       <c r="O45" s="6">
-        <v>90.57</v>
+        <v>95.616</v>
       </c>
       <c r="Q45" s="6">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="R45" s="6">
-        <v>11.774100000000001</v>
+        <v>9.5616000000000003</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6">
-        <v>100036</v>
+        <v>100045</v>
       </c>
       <c r="B46" s="7">
-        <v>42712</v>
+        <v>42440</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>87</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>140</v>
+        <v>191</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>8</v>
@@ -4635,178 +4653,169 @@
         <v>3</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>6</v>
+        <v>193</v>
       </c>
       <c r="J46" s="6">
-        <v>75080</v>
+        <v>55122</v>
       </c>
       <c r="K46" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L46" s="6" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="M46" s="6" t="s">
         <v>208</v>
       </c>
       <c r="N46" s="6" t="s">
-        <v>31</v>
+        <v>206</v>
       </c>
       <c r="O46" s="6">
-        <v>1097.5440000000001</v>
+        <v>45.98</v>
       </c>
       <c r="P46" s="6">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="Q46" s="6">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="R46" s="6">
-        <v>123.47369999999999</v>
+        <v>19.7714</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6">
-        <v>100041</v>
+        <v>100046</v>
       </c>
       <c r="B47" s="7">
-        <v>42365</v>
+        <v>42440</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>143</v>
+        <v>190</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>144</v>
+        <v>191</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="G47" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>146</v>
+        <v>192</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>6</v>
+        <v>193</v>
       </c>
       <c r="J47" s="6">
-        <v>77041</v>
+        <v>55122</v>
       </c>
       <c r="K47" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L47" s="6" t="s">
-        <v>209</v>
+        <v>194</v>
       </c>
       <c r="M47" s="6" t="s">
-        <v>208</v>
+        <v>40</v>
       </c>
       <c r="O47" s="6">
-        <v>371.16800000000001</v>
-      </c>
-      <c r="P47" s="6">
-        <v>4</v>
+        <v>17.46</v>
       </c>
       <c r="Q47" s="6">
-        <v>0.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6">
-        <v>100042</v>
+        <v>100047</v>
       </c>
       <c r="B48" s="7">
-        <v>42988</v>
+        <v>41932</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>86</v>
+        <v>111</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>210</v>
+        <v>195</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="J48" s="6">
-        <v>60540</v>
+        <v>48185</v>
       </c>
       <c r="K48" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="M48" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="N48" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P48" s="6">
-        <v>4</v>
+        <v>40</v>
+      </c>
+      <c r="O48" s="6">
+        <v>211.96</v>
       </c>
       <c r="Q48" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="R48" s="6">
-        <v>16.5564</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6">
-        <v>100045</v>
+        <v>100048</v>
       </c>
       <c r="B49" s="7">
-        <v>42440</v>
+        <v>42541</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>190</v>
+        <v>215</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>191</v>
+        <v>216</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>3</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>192</v>
+        <v>217</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>193</v>
+        <v>218</v>
       </c>
       <c r="J49" s="6">
-        <v>55122</v>
+        <v>19901</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="M49" s="6" t="s">
         <v>208</v>
@@ -4815,21 +4824,21 @@
         <v>206</v>
       </c>
       <c r="O49" s="6">
-        <v>45.98</v>
+        <v>45</v>
       </c>
       <c r="P49" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q49" s="6">
         <v>0</v>
       </c>
       <c r="R49" s="6">
-        <v>19.7714</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="50" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="6">
-        <v>100048</v>
+        <v>100049</v>
       </c>
       <c r="B50" s="7">
         <v>42541</v>
@@ -4862,42 +4871,36 @@
         <v>129</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="M50" s="6" t="s">
         <v>208</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="O50" s="6">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="P50" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q50" s="6">
         <v>0</v>
       </c>
-      <c r="R50" s="6">
-        <v>4.95</v>
-      </c>
     </row>
     <row r="51" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="6">
-        <v>100049</v>
+        <v>100050</v>
       </c>
       <c r="B51" s="7">
-        <v>42541</v>
+        <v>42112</v>
       </c>
       <c r="C51" s="6" t="s">
         <v>86</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>4</v>
@@ -4906,28 +4909,25 @@
         <v>3</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="J51" s="6">
-        <v>19901</v>
+        <v>47150</v>
       </c>
       <c r="K51" s="6" t="s">
-        <v>129</v>
+        <v>0</v>
       </c>
       <c r="L51" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="M51" s="6" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="N51" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P51" s="6">
-        <v>2</v>
+        <v>44</v>
+      </c>
+      <c r="O51" s="6">
+        <v>38.22</v>
       </c>
       <c r="Q51" s="6">
         <v>0</v>
@@ -34768,7 +34768,7 @@
   </sheetData>
   <autoFilter ref="A1:R1" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R51">
-      <sortCondition ref="M1"/>
+      <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>